<commit_message>
Completely refactored the basic balancing of openIO. Also properly integrated the endogenization feature.
</commit_message>
<xml_diff>
--- a/Data/Concordances/Endogenizing.xlsx
+++ b/Data/Concordances/Endogenizing.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\Concordances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09A728F6-F1AB-4563-8FBF-471FAE944805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF7C559-75B8-417F-8928-6A2503603A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="507">
   <si>
     <t>Mining and quarrying (except oil and gas)</t>
   </si>
@@ -303,9 +314,6 @@
     <t>Water, sewage and other systems</t>
   </si>
   <si>
-    <t>Residential building construction</t>
-  </si>
-  <si>
     <t>Non-residential building construction</t>
   </si>
   <si>
@@ -892,9 +900,6 @@
   </si>
   <si>
     <t>BS221300</t>
-  </si>
-  <si>
-    <t>BS23A000</t>
   </si>
   <si>
     <t>BS23B000</t>
@@ -1904,10 +1909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADE6630-C47D-4A62-A208-F303F1F877D2}">
-  <dimension ref="A1:C235"/>
+  <dimension ref="A1:C234"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1919,18 +1924,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>506</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B2" t="s">
         <v>70</v>
@@ -1941,7 +1946,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
         <v>71</v>
@@ -1952,7 +1957,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B4" t="s">
         <v>72</v>
@@ -1963,7 +1968,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B5" t="s">
         <v>73</v>
@@ -1974,7 +1979,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
         <v>74</v>
@@ -1985,7 +1990,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B7" t="s">
         <v>75</v>
@@ -1996,7 +2001,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -2007,7 +2012,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -2018,7 +2023,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B10" t="s">
         <v>76</v>
@@ -2029,7 +2034,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B11" t="s">
         <v>77</v>
@@ -2040,7 +2045,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B12" t="s">
         <v>33</v>
@@ -2051,7 +2056,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -2062,7 +2067,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B14" t="s">
         <v>78</v>
@@ -2073,7 +2078,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B15" t="s">
         <v>79</v>
@@ -2084,7 +2089,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B16" t="s">
         <v>80</v>
@@ -2095,7 +2100,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B17" t="s">
         <v>81</v>
@@ -2106,7 +2111,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B18" t="s">
         <v>82</v>
@@ -2117,7 +2122,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s">
         <v>83</v>
@@ -2128,7 +2133,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B20" t="s">
         <v>84</v>
@@ -2139,7 +2144,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B21" t="s">
         <v>85</v>
@@ -2150,7 +2155,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B22" t="s">
         <v>86</v>
@@ -2161,7 +2166,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B23" t="s">
         <v>87</v>
@@ -2172,7 +2177,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B24" t="s">
         <v>88</v>
@@ -2183,7 +2188,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
@@ -2194,7 +2199,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B26" t="s">
         <v>90</v>
@@ -2205,7 +2210,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
@@ -2216,7 +2221,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B28" t="s">
         <v>91</v>
@@ -2227,7 +2232,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B29" t="s">
         <v>92</v>
@@ -2238,7 +2243,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B30" t="s">
         <v>93</v>
@@ -2249,7 +2254,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31" t="s">
         <v>94</v>
@@ -2260,7 +2265,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B32" t="s">
         <v>95</v>
@@ -2271,7 +2276,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B33" t="s">
         <v>96</v>
@@ -2282,7 +2287,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B34" t="s">
         <v>97</v>
@@ -2293,7 +2298,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B35" t="s">
         <v>98</v>
@@ -2304,7 +2309,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B36" t="s">
         <v>99</v>
@@ -2315,18 +2320,18 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B37" t="s">
         <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B38" t="s">
         <v>101</v>
@@ -2337,7 +2342,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B39" t="s">
         <v>102</v>
@@ -2348,7 +2353,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B40" t="s">
         <v>103</v>
@@ -2359,7 +2364,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B41" t="s">
         <v>104</v>
@@ -2370,7 +2375,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B42" t="s">
         <v>105</v>
@@ -2381,7 +2386,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B43" t="s">
         <v>106</v>
@@ -2392,7 +2397,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B44" t="s">
         <v>107</v>
@@ -2403,7 +2408,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B45" t="s">
         <v>108</v>
@@ -2414,18 +2419,18 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B46" t="s">
         <v>109</v>
       </c>
       <c r="C46" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B47" t="s">
         <v>110</v>
@@ -2436,7 +2441,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B48" t="s">
         <v>111</v>
@@ -2447,7 +2452,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B49" t="s">
         <v>112</v>
@@ -2458,40 +2463,40 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B50" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B51" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B53" t="s">
         <v>114</v>
@@ -2502,7 +2507,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B54" t="s">
         <v>115</v>
@@ -2513,18 +2518,18 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B55" t="s">
         <v>116</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B56" t="s">
         <v>117</v>
@@ -2535,29 +2540,29 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="C58" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s">
         <v>119</v>
@@ -2568,18 +2573,18 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B60" t="s">
         <v>120</v>
       </c>
       <c r="C60" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B61" t="s">
         <v>121</v>
@@ -2590,7 +2595,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B62" t="s">
         <v>122</v>
@@ -2601,7 +2606,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B63" t="s">
         <v>123</v>
@@ -2612,7 +2617,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B64" t="s">
         <v>124</v>
@@ -2623,7 +2628,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B65" t="s">
         <v>125</v>
@@ -2634,7 +2639,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B66" t="s">
         <v>126</v>
@@ -2645,18 +2650,18 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B67" t="s">
         <v>127</v>
       </c>
       <c r="C67" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B68" t="s">
         <v>128</v>
@@ -2667,18 +2672,18 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B69" t="s">
         <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B70" t="s">
         <v>130</v>
@@ -2689,18 +2694,18 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B71" t="s">
         <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B72" t="s">
         <v>132</v>
@@ -2711,7 +2716,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B73" t="s">
         <v>133</v>
@@ -2722,7 +2727,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B74" t="s">
         <v>134</v>
@@ -2733,7 +2738,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B75" t="s">
         <v>135</v>
@@ -2744,18 +2749,18 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B76" t="s">
         <v>136</v>
       </c>
       <c r="C76" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B77" t="s">
         <v>137</v>
@@ -2766,7 +2771,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B78" t="s">
         <v>138</v>
@@ -2777,7 +2782,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B79" t="s">
         <v>139</v>
@@ -2788,7 +2793,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B80" t="s">
         <v>140</v>
@@ -2799,7 +2804,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B81" t="s">
         <v>141</v>
@@ -2810,7 +2815,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B82" t="s">
         <v>142</v>
@@ -2821,7 +2826,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B83" t="s">
         <v>143</v>
@@ -2832,18 +2837,18 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B84" t="s">
         <v>144</v>
       </c>
       <c r="C84" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B85" t="s">
         <v>145</v>
@@ -2854,7 +2859,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B86" t="s">
         <v>146</v>
@@ -2865,7 +2870,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B87" t="s">
         <v>147</v>
@@ -2876,7 +2881,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B88" t="s">
         <v>148</v>
@@ -2887,7 +2892,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B89" t="s">
         <v>149</v>
@@ -2898,7 +2903,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B90" t="s">
         <v>150</v>
@@ -2909,18 +2914,18 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B91" t="s">
         <v>151</v>
       </c>
       <c r="C91" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B92" t="s">
         <v>152</v>
@@ -2931,7 +2936,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B93" t="s">
         <v>153</v>
@@ -2942,7 +2947,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B94" t="s">
         <v>154</v>
@@ -2953,18 +2958,18 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B95" t="s">
         <v>155</v>
       </c>
       <c r="C95" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B96" t="s">
         <v>156</v>
@@ -2975,7 +2980,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B97" t="s">
         <v>157</v>
@@ -2986,7 +2991,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B98" t="s">
         <v>158</v>
@@ -2997,18 +3002,18 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B99" t="s">
         <v>159</v>
       </c>
       <c r="C99" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B100" t="s">
         <v>160</v>
@@ -3019,7 +3024,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B101" t="s">
         <v>161</v>
@@ -3030,7 +3035,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B102" t="s">
         <v>162</v>
@@ -3041,7 +3046,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B103" t="s">
         <v>163</v>
@@ -3052,7 +3057,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B104" t="s">
         <v>164</v>
@@ -3063,7 +3068,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B105" t="s">
         <v>165</v>
@@ -3074,7 +3079,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B106" t="s">
         <v>166</v>
@@ -3085,7 +3090,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B107" t="s">
         <v>167</v>
@@ -3096,7 +3101,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B108" t="s">
         <v>168</v>
@@ -3107,7 +3112,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B109" t="s">
         <v>169</v>
@@ -3118,7 +3123,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B110" t="s">
         <v>170</v>
@@ -3129,7 +3134,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B111" t="s">
         <v>171</v>
@@ -3140,7 +3145,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B112" t="s">
         <v>172</v>
@@ -3151,7 +3156,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B113" t="s">
         <v>173</v>
@@ -3162,18 +3167,18 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B114" t="s">
         <v>174</v>
       </c>
       <c r="C114" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B115" t="s">
         <v>175</v>
@@ -3184,7 +3189,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B116" t="s">
         <v>176</v>
@@ -3195,18 +3200,18 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B117" t="s">
         <v>177</v>
       </c>
       <c r="C117" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B118" t="s">
         <v>178</v>
@@ -3217,18 +3222,18 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B119" t="s">
         <v>179</v>
       </c>
       <c r="C119" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B120" t="s">
         <v>180</v>
@@ -3239,7 +3244,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B121" t="s">
         <v>181</v>
@@ -3250,7 +3255,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B122" t="s">
         <v>182</v>
@@ -3261,7 +3266,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B123" t="s">
         <v>183</v>
@@ -3272,7 +3277,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B124" t="s">
         <v>184</v>
@@ -3283,7 +3288,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B125" t="s">
         <v>185</v>
@@ -3294,7 +3299,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B126" t="s">
         <v>186</v>
@@ -3305,7 +3310,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B127" t="s">
         <v>187</v>
@@ -3316,18 +3321,18 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B128" t="s">
         <v>188</v>
       </c>
       <c r="C128" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B129" t="s">
         <v>189</v>
@@ -3338,7 +3343,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B130" t="s">
         <v>190</v>
@@ -3349,7 +3354,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B131" t="s">
         <v>191</v>
@@ -3360,7 +3365,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B132" t="s">
         <v>192</v>
@@ -3371,7 +3376,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B133" t="s">
         <v>193</v>
@@ -3382,7 +3387,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B134" t="s">
         <v>194</v>
@@ -3393,7 +3398,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B135" t="s">
         <v>195</v>
@@ -3404,7 +3409,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B136" t="s">
         <v>196</v>
@@ -3415,7 +3420,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B137" t="s">
         <v>197</v>
@@ -3426,7 +3431,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B138" t="s">
         <v>198</v>
@@ -3437,7 +3442,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B139" t="s">
         <v>199</v>
@@ -3448,7 +3453,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B140" t="s">
         <v>200</v>
@@ -3459,7 +3464,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B141" t="s">
         <v>201</v>
@@ -3470,18 +3475,18 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B142" t="s">
         <v>202</v>
       </c>
       <c r="C142" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B143" t="s">
         <v>203</v>
@@ -3492,7 +3497,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B144" t="s">
         <v>204</v>
@@ -3503,7 +3508,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B145" t="s">
         <v>205</v>
@@ -3514,7 +3519,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B146" t="s">
         <v>206</v>
@@ -3525,7 +3530,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B147" t="s">
         <v>207</v>
@@ -3536,7 +3541,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B148" t="s">
         <v>208</v>
@@ -3547,7 +3552,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B149" t="s">
         <v>209</v>
@@ -3558,7 +3563,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B150" t="s">
         <v>210</v>
@@ -3569,7 +3574,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B151" t="s">
         <v>211</v>
@@ -3580,7 +3585,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B152" t="s">
         <v>212</v>
@@ -3591,7 +3596,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B153" t="s">
         <v>213</v>
@@ -3602,7 +3607,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B154" t="s">
         <v>214</v>
@@ -3613,18 +3618,18 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B155" t="s">
         <v>215</v>
       </c>
       <c r="C155" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B156" t="s">
         <v>216</v>
@@ -3635,7 +3640,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B157" t="s">
         <v>217</v>
@@ -3646,7 +3651,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B158" t="s">
         <v>218</v>
@@ -3657,7 +3662,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B159" t="s">
         <v>219</v>
@@ -3668,7 +3673,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B160" t="s">
         <v>220</v>
@@ -3679,7 +3684,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B161" t="s">
         <v>221</v>
@@ -3690,7 +3695,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B162" t="s">
         <v>222</v>
@@ -3701,7 +3706,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B163" t="s">
         <v>223</v>
@@ -3712,7 +3717,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B164" t="s">
         <v>224</v>
@@ -3723,10 +3728,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B165" t="s">
-        <v>225</v>
+        <v>54</v>
       </c>
       <c r="C165" t="s">
         <v>35</v>
@@ -3734,18 +3739,18 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B166" t="s">
-        <v>54</v>
+        <v>225</v>
       </c>
       <c r="C166" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B167" t="s">
         <v>226</v>
@@ -3756,7 +3761,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B168" t="s">
         <v>227</v>
@@ -3767,7 +3772,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B169" t="s">
         <v>228</v>
@@ -3778,7 +3783,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B170" t="s">
         <v>229</v>
@@ -3789,7 +3794,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B171" t="s">
         <v>230</v>
@@ -3800,7 +3805,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B172" t="s">
         <v>231</v>
@@ -3811,7 +3816,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B173" t="s">
         <v>232</v>
@@ -3822,18 +3827,18 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B174" t="s">
         <v>233</v>
       </c>
       <c r="C174" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B175" t="s">
         <v>234</v>
@@ -3844,7 +3849,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B176" t="s">
         <v>235</v>
@@ -3855,7 +3860,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B177" t="s">
         <v>236</v>
@@ -3866,7 +3871,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B178" t="s">
         <v>237</v>
@@ -3877,7 +3882,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B179" t="s">
         <v>238</v>
@@ -3888,21 +3893,21 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B180" t="s">
-        <v>239</v>
+        <v>55</v>
       </c>
       <c r="C180" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B181" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C181" t="s">
         <v>44</v>
@@ -3910,10 +3915,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B182" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C182" t="s">
         <v>44</v>
@@ -3921,10 +3926,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B183" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C183" t="s">
         <v>44</v>
@@ -3932,10 +3937,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B184" t="s">
-        <v>58</v>
+        <v>239</v>
       </c>
       <c r="C184" t="s">
         <v>44</v>
@@ -3943,10 +3948,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B185" t="s">
-        <v>240</v>
+        <v>59</v>
       </c>
       <c r="C185" t="s">
         <v>44</v>
@@ -3954,10 +3959,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B186" t="s">
-        <v>59</v>
+        <v>240</v>
       </c>
       <c r="C186" t="s">
         <v>44</v>
@@ -3965,10 +3970,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B187" t="s">
-        <v>241</v>
+        <v>60</v>
       </c>
       <c r="C187" t="s">
         <v>44</v>
@@ -3976,10 +3981,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B188" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C188" t="s">
         <v>44</v>
@@ -3987,32 +3992,32 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B189" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C189" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B190" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C190" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B191" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C191" t="s">
         <v>13</v>
@@ -4020,10 +4025,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B192" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C192" t="s">
         <v>13</v>
@@ -4031,10 +4036,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B193" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C193" t="s">
         <v>13</v>
@@ -4042,10 +4047,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B194" t="s">
-        <v>64</v>
+        <v>241</v>
       </c>
       <c r="C194" t="s">
         <v>13</v>
@@ -4053,10 +4058,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B195" t="s">
-        <v>242</v>
+        <v>65</v>
       </c>
       <c r="C195" t="s">
         <v>13</v>
@@ -4064,10 +4069,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B196" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C196" t="s">
         <v>13</v>
@@ -4075,10 +4080,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B197" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C197" t="s">
         <v>13</v>
@@ -4086,29 +4091,29 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B198" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C198" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B199" t="s">
-        <v>41</v>
+        <v>242</v>
       </c>
       <c r="C199" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B200" t="s">
         <v>243</v>
@@ -4119,7 +4124,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B201" t="s">
         <v>244</v>
@@ -4130,10 +4135,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B202" t="s">
-        <v>245</v>
+        <v>494</v>
       </c>
       <c r="C202" t="s">
         <v>52</v>
@@ -4141,10 +4146,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B203" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C203" t="s">
         <v>52</v>
@@ -4152,18 +4157,18 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B204" t="s">
-        <v>497</v>
+        <v>245</v>
       </c>
       <c r="C204" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B205" t="s">
         <v>246</v>
@@ -4174,7 +4179,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B206" t="s">
         <v>247</v>
@@ -4185,18 +4190,18 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B207" t="s">
         <v>248</v>
       </c>
       <c r="C207" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B208" t="s">
         <v>249</v>
@@ -4207,7 +4212,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B209" t="s">
         <v>250</v>
@@ -4218,18 +4223,18 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B210" t="s">
         <v>251</v>
       </c>
       <c r="C210" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B211" t="s">
         <v>252</v>
@@ -4240,7 +4245,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B212" t="s">
         <v>253</v>
@@ -4251,10 +4256,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B213" t="s">
-        <v>254</v>
+        <v>69</v>
       </c>
       <c r="C213" t="s">
         <v>8</v>
@@ -4262,10 +4267,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B214" t="s">
-        <v>69</v>
+        <v>254</v>
       </c>
       <c r="C214" t="s">
         <v>8</v>
@@ -4273,7 +4278,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B215" t="s">
         <v>255</v>
@@ -4284,7 +4289,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B216" t="s">
         <v>256</v>
@@ -4295,21 +4300,21 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B217" t="s">
-        <v>257</v>
+        <v>496</v>
       </c>
       <c r="C217" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B218" t="s">
-        <v>498</v>
+        <v>257</v>
       </c>
       <c r="C218" t="s">
         <v>3</v>
@@ -4317,10 +4322,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B219" t="s">
-        <v>258</v>
+        <v>497</v>
       </c>
       <c r="C219" t="s">
         <v>3</v>
@@ -4328,10 +4333,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B220" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C220" t="s">
         <v>3</v>
@@ -4339,10 +4344,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B221" t="s">
-        <v>500</v>
+        <v>258</v>
       </c>
       <c r="C221" t="s">
         <v>3</v>
@@ -4350,7 +4355,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B222" t="s">
         <v>259</v>
@@ -4361,7 +4366,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B223" t="s">
         <v>260</v>
@@ -4372,21 +4377,21 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B224" t="s">
-        <v>261</v>
+        <v>499</v>
       </c>
       <c r="C224" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B225" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C225" t="s">
         <v>16</v>
@@ -4394,10 +4399,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B226" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C226" t="s">
         <v>16</v>
@@ -4405,10 +4410,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B227" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C227" t="s">
         <v>16</v>
@@ -4416,89 +4421,78 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B228" t="s">
-        <v>504</v>
+        <v>6</v>
       </c>
       <c r="C228" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B229" t="s">
-        <v>6</v>
+        <v>503</v>
       </c>
       <c r="C229" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B230" t="s">
-        <v>505</v>
+        <v>27</v>
       </c>
       <c r="C230" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B231" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C231" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B232" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C232" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B233" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C233" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B234" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="C234" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A235" t="s">
-        <v>495</v>
-      </c>
-      <c r="B235" t="s">
-        <v>34</v>
-      </c>
-      <c r="C235" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>